<commit_message>
update data and methods
</commit_message>
<xml_diff>
--- a/China_Acc_Results/Result/city_gdponly.xlsx
+++ b/China_Acc_Results/Result/city_gdponly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectpolyu-my.sharepoint.com/personal/24046865g_connect_polyu_hk/Documents/Student Assistant/ChinaDynam/China_Acc_Results/Result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="212" documentId="13_ncr:1_{400FA808-2CCC-4299-A240-85E9D0297A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B226CF6-8B09-45F3-B998-D071CB101CDD}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="13_ncr:1_{400FA808-2CCC-4299-A240-85E9D0297A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{591D88A4-DF63-4C92-8C29-72424DA67336}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1772,10 +1772,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AJ370"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I225" sqref="I225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -1897,7 +1898,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>40</v>
       </c>
@@ -1987,7 +1988,7 @@
       <c r="AI2" s="2"/>
       <c r="AJ2" s="2"/>
     </row>
-    <row r="3" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -2093,7 +2094,7 @@
       </c>
       <c r="AJ3" s="2"/>
     </row>
-    <row r="4" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -2189,7 +2190,7 @@
         <v>9083.6200000000008</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>50</v>
       </c>
@@ -2277,7 +2278,7 @@
         <v>9662.48</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>56</v>
       </c>
@@ -2367,7 +2368,7 @@
         <v>7275.66</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>60</v>
       </c>
@@ -2463,7 +2464,7 @@
         <v>3200.33</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>64</v>
       </c>
@@ -2543,7 +2544,7 @@
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
     </row>
-    <row r="9" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>62</v>
       </c>
@@ -2631,7 +2632,7 @@
       <c r="AI9" s="2"/>
       <c r="AJ9" s="2"/>
     </row>
-    <row r="10" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>66</v>
       </c>
@@ -2707,7 +2708,7 @@
       <c r="AI10" s="2"/>
       <c r="AJ10" s="2"/>
     </row>
-    <row r="11" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>75</v>
       </c>
@@ -2783,7 +2784,7 @@
       <c r="AI11" s="2"/>
       <c r="AJ11" s="2"/>
     </row>
-    <row r="12" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>59</v>
       </c>
@@ -2873,7 +2874,7 @@
         <v>4297.58</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>68</v>
       </c>
@@ -2965,7 +2966,7 @@
         <v>3209.1</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>67</v>
       </c>
@@ -3045,7 +3046,7 @@
       <c r="AI14" s="2"/>
       <c r="AJ14" s="2"/>
     </row>
-    <row r="15" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>65</v>
       </c>
@@ -3121,7 +3122,7 @@
       <c r="AI15" s="2"/>
       <c r="AJ15" s="2"/>
     </row>
-    <row r="16" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>91</v>
       </c>
@@ -3199,7 +3200,7 @@
       <c r="AI16" s="2"/>
       <c r="AJ16" s="2"/>
     </row>
-    <row r="17" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>86</v>
       </c>
@@ -3273,7 +3274,7 @@
       <c r="AI17" s="2"/>
       <c r="AJ17" s="2"/>
     </row>
-    <row r="18" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>71</v>
       </c>
@@ -3349,7 +3350,7 @@
       <c r="AI18" s="2"/>
       <c r="AJ18" s="2"/>
     </row>
-    <row r="19" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>76</v>
       </c>
@@ -3433,7 +3434,7 @@
       <c r="AI19" s="2"/>
       <c r="AJ19" s="2"/>
     </row>
-    <row r="20" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>78</v>
       </c>
@@ -3511,7 +3512,7 @@
       <c r="AI20" s="2"/>
       <c r="AJ20" s="2"/>
     </row>
-    <row r="21" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>110</v>
       </c>
@@ -3597,7 +3598,7 @@
         <v>3345.94</v>
       </c>
     </row>
-    <row r="22" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>79</v>
       </c>
@@ -3681,7 +3682,7 @@
       <c r="AI22" s="2"/>
       <c r="AJ22" s="2"/>
     </row>
-    <row r="23" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>92</v>
       </c>
@@ -3771,7 +3772,7 @@
         <v>3807.31</v>
       </c>
     </row>
-    <row r="24" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>87</v>
       </c>
@@ -3847,7 +3848,7 @@
       <c r="AI24" s="2"/>
       <c r="AJ24" s="2"/>
     </row>
-    <row r="25" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>84</v>
       </c>
@@ -3933,7 +3934,7 @@
       <c r="AI25" s="2"/>
       <c r="AJ25" s="2"/>
     </row>
-    <row r="26" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>81</v>
       </c>
@@ -4025,7 +4026,7 @@
         <v>1863.21</v>
       </c>
     </row>
-    <row r="27" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>97</v>
       </c>
@@ -4103,7 +4104,7 @@
       <c r="AI27" s="2"/>
       <c r="AJ27" s="2"/>
     </row>
-    <row r="28" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>80</v>
       </c>
@@ -4195,7 +4196,7 @@
         <v>1430.4</v>
       </c>
     </row>
-    <row r="29" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>93</v>
       </c>
@@ -4281,7 +4282,7 @@
       <c r="AI29" s="2"/>
       <c r="AJ29" s="2"/>
     </row>
-    <row r="30" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>69</v>
       </c>
@@ -4355,7 +4356,7 @@
       <c r="AI30" s="2"/>
       <c r="AJ30" s="2"/>
     </row>
-    <row r="31" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>83</v>
       </c>
@@ -4431,7 +4432,7 @@
       <c r="AI31" s="2"/>
       <c r="AJ31" s="2"/>
     </row>
-    <row r="32" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>72</v>
       </c>
@@ -4505,7 +4506,7 @@
       <c r="AI32" s="2"/>
       <c r="AJ32" s="2"/>
     </row>
-    <row r="33" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>109</v>
       </c>
@@ -4585,7 +4586,7 @@
       <c r="AI33" s="2"/>
       <c r="AJ33" s="2"/>
     </row>
-    <row r="34" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>95</v>
       </c>
@@ -4663,7 +4664,7 @@
       <c r="AI34" s="2"/>
       <c r="AJ34" s="2"/>
     </row>
-    <row r="35" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>88</v>
       </c>
@@ -4743,7 +4744,7 @@
       <c r="AI35" s="2"/>
       <c r="AJ35" s="2"/>
     </row>
-    <row r="36" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>89</v>
       </c>
@@ -4817,7 +4818,7 @@
       <c r="AI36" s="2"/>
       <c r="AJ36" s="2"/>
     </row>
-    <row r="37" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>77</v>
       </c>
@@ -4891,7 +4892,7 @@
       <c r="AI37" s="2"/>
       <c r="AJ37" s="2"/>
     </row>
-    <row r="38" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>112</v>
       </c>
@@ -4965,7 +4966,7 @@
       <c r="AI38" s="2"/>
       <c r="AJ38" s="2"/>
     </row>
-    <row r="39" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>102</v>
       </c>
@@ -5041,7 +5042,7 @@
       <c r="AI39" s="2"/>
       <c r="AJ39" s="2"/>
     </row>
-    <row r="40" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>286</v>
       </c>
@@ -5117,7 +5118,7 @@
       <c r="AI40" s="2"/>
       <c r="AJ40" s="2"/>
     </row>
-    <row r="41" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>105</v>
       </c>
@@ -5197,7 +5198,7 @@
       <c r="AI41" s="2"/>
       <c r="AJ41" s="2"/>
     </row>
-    <row r="42" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>85</v>
       </c>
@@ -5289,7 +5290,7 @@
         <v>1915.05</v>
       </c>
     </row>
-    <row r="43" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>122</v>
       </c>
@@ -5367,7 +5368,7 @@
       <c r="AI43" s="2"/>
       <c r="AJ43" s="2"/>
     </row>
-    <row r="44" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>96</v>
       </c>
@@ -5457,7 +5458,7 @@
       <c r="AI44" s="2"/>
       <c r="AJ44" s="2"/>
     </row>
-    <row r="45" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>101</v>
       </c>
@@ -5533,7 +5534,7 @@
       <c r="AI45" s="2"/>
       <c r="AJ45" s="2"/>
     </row>
-    <row r="46" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>107</v>
       </c>
@@ -5613,7 +5614,7 @@
       <c r="AI46" s="2"/>
       <c r="AJ46" s="2"/>
     </row>
-    <row r="47" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>244</v>
       </c>
@@ -5703,7 +5704,7 @@
       <c r="AI47" s="2"/>
       <c r="AJ47" s="2"/>
     </row>
-    <row r="48" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>121</v>
       </c>
@@ -5779,7 +5780,7 @@
       <c r="AI48" s="2"/>
       <c r="AJ48" s="2"/>
     </row>
-    <row r="49" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>125</v>
       </c>
@@ -5853,7 +5854,7 @@
       <c r="AI49" s="2"/>
       <c r="AJ49" s="2"/>
     </row>
-    <row r="50" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>111</v>
       </c>
@@ -5939,7 +5940,7 @@
       <c r="AI50" s="2"/>
       <c r="AJ50" s="2"/>
     </row>
-    <row r="51" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>117</v>
       </c>
@@ -6013,7 +6014,7 @@
       <c r="AI51" s="2"/>
       <c r="AJ51" s="2"/>
     </row>
-    <row r="52" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>82</v>
       </c>
@@ -6103,7 +6104,7 @@
         <v>1588.7</v>
       </c>
     </row>
-    <row r="53" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>134</v>
       </c>
@@ -6183,7 +6184,7 @@
       <c r="AI53" s="2"/>
       <c r="AJ53" s="2"/>
     </row>
-    <row r="54" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>99</v>
       </c>
@@ -6275,7 +6276,7 @@
         <v>998.96</v>
       </c>
     </row>
-    <row r="55" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>119</v>
       </c>
@@ -6365,7 +6366,7 @@
       <c r="AI55" s="2"/>
       <c r="AJ55" s="2"/>
     </row>
-    <row r="56" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>126</v>
       </c>
@@ -6455,7 +6456,7 @@
         <v>1448.95</v>
       </c>
     </row>
-    <row r="57" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>115</v>
       </c>
@@ -6529,7 +6530,7 @@
       <c r="AI57" s="2"/>
       <c r="AJ57" s="2"/>
     </row>
-    <row r="58" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>162</v>
       </c>
@@ -6607,7 +6608,7 @@
       <c r="AI58" s="2"/>
       <c r="AJ58" s="2"/>
     </row>
-    <row r="59" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>151</v>
       </c>
@@ -6681,7 +6682,7 @@
       <c r="AI59" s="2"/>
       <c r="AJ59" s="2"/>
     </row>
-    <row r="60" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>130</v>
       </c>
@@ -6773,7 +6774,7 @@
         <v>1228.82</v>
       </c>
     </row>
-    <row r="61" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>196</v>
       </c>
@@ -6861,7 +6862,7 @@
       <c r="AI61" s="2"/>
       <c r="AJ61" s="2"/>
     </row>
-    <row r="62" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>157</v>
       </c>
@@ -6945,7 +6946,7 @@
       <c r="AI62" s="2"/>
       <c r="AJ62" s="2"/>
     </row>
-    <row r="63" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>199</v>
       </c>
@@ -7035,7 +7036,7 @@
         <v>818.47</v>
       </c>
     </row>
-    <row r="64" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>106</v>
       </c>
@@ -7111,7 +7112,7 @@
       <c r="AI64" s="2"/>
       <c r="AJ64" s="2"/>
     </row>
-    <row r="65" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>94</v>
       </c>
@@ -7185,7 +7186,7 @@
       <c r="AI65" s="2"/>
       <c r="AJ65" s="2"/>
     </row>
-    <row r="66" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>189</v>
       </c>
@@ -7261,7 +7262,7 @@
       <c r="AI66" s="2"/>
       <c r="AJ66" s="2"/>
     </row>
-    <row r="67" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>114</v>
       </c>
@@ -7353,7 +7354,7 @@
         <v>911.6</v>
       </c>
     </row>
-    <row r="68" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>195</v>
       </c>
@@ -7431,7 +7432,7 @@
       <c r="AI68" s="2"/>
       <c r="AJ68" s="2"/>
     </row>
-    <row r="69" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>133</v>
       </c>
@@ -7509,7 +7510,7 @@
       <c r="AI69" s="2"/>
       <c r="AJ69" s="2"/>
     </row>
-    <row r="70" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>103</v>
       </c>
@@ -7599,7 +7600,7 @@
       <c r="AI70" s="2"/>
       <c r="AJ70" s="2"/>
     </row>
-    <row r="71" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>150</v>
       </c>
@@ -7673,7 +7674,7 @@
       <c r="AI71" s="2"/>
       <c r="AJ71" s="2"/>
     </row>
-    <row r="72" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>181</v>
       </c>
@@ -7747,7 +7748,7 @@
       <c r="AI72" s="2"/>
       <c r="AJ72" s="2"/>
     </row>
-    <row r="73" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>137</v>
       </c>
@@ -7831,7 +7832,7 @@
       <c r="AI73" s="2"/>
       <c r="AJ73" s="2"/>
     </row>
-    <row r="74" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>132</v>
       </c>
@@ -7921,7 +7922,7 @@
         <v>1137.8499999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>158</v>
       </c>
@@ -8009,7 +8010,7 @@
         <v>1115.6500000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>185</v>
       </c>
@@ -8091,7 +8092,7 @@
       <c r="AI76" s="2"/>
       <c r="AJ76" s="2"/>
     </row>
-    <row r="77" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>140</v>
       </c>
@@ -8173,7 +8174,7 @@
       <c r="AI77" s="2"/>
       <c r="AJ77" s="2"/>
     </row>
-    <row r="78" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>108</v>
       </c>
@@ -8257,7 +8258,7 @@
       <c r="AI78" s="2"/>
       <c r="AJ78" s="2"/>
     </row>
-    <row r="79" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>138</v>
       </c>
@@ -8343,7 +8344,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="80" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>90</v>
       </c>
@@ -8435,7 +8436,7 @@
       <c r="AI80" s="2"/>
       <c r="AJ80" s="2"/>
     </row>
-    <row r="81" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>120</v>
       </c>
@@ -8523,7 +8524,7 @@
       <c r="AI81" s="2"/>
       <c r="AJ81" s="2"/>
     </row>
-    <row r="82" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>113</v>
       </c>
@@ -8615,7 +8616,7 @@
       <c r="AI82" s="2"/>
       <c r="AJ82" s="2"/>
     </row>
-    <row r="83" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>135</v>
       </c>
@@ -8707,7 +8708,7 @@
         <v>693.83</v>
       </c>
     </row>
-    <row r="84" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>193</v>
       </c>
@@ -8795,7 +8796,7 @@
       <c r="AI84" s="2"/>
       <c r="AJ84" s="2"/>
     </row>
-    <row r="85" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>194</v>
       </c>
@@ -8873,7 +8874,7 @@
       <c r="AI85" s="2"/>
       <c r="AJ85" s="2"/>
     </row>
-    <row r="86" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>131</v>
       </c>
@@ -8947,7 +8948,7 @@
       <c r="AI86" s="2"/>
       <c r="AJ86" s="2"/>
     </row>
-    <row r="87" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>213</v>
       </c>
@@ -9043,7 +9044,7 @@
         <v>1214.98</v>
       </c>
     </row>
-    <row r="88" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>127</v>
       </c>
@@ -9137,7 +9138,7 @@
         <v>633.84</v>
       </c>
     </row>
-    <row r="89" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>178</v>
       </c>
@@ -9211,7 +9212,7 @@
       <c r="AI89" s="2"/>
       <c r="AJ89" s="2"/>
     </row>
-    <row r="90" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>148</v>
       </c>
@@ -9301,7 +9302,7 @@
       <c r="AI90" s="2"/>
       <c r="AJ90" s="2"/>
     </row>
-    <row r="91" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>129</v>
       </c>
@@ -9379,7 +9380,7 @@
       <c r="AI91" s="2"/>
       <c r="AJ91" s="2"/>
     </row>
-    <row r="92" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>100</v>
       </c>
@@ -9457,7 +9458,7 @@
       <c r="AI92" s="2"/>
       <c r="AJ92" s="2"/>
     </row>
-    <row r="93" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>143</v>
       </c>
@@ -9549,7 +9550,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="94" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>208</v>
       </c>
@@ -9635,7 +9636,7 @@
         <v>689.51</v>
       </c>
     </row>
-    <row r="95" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>217</v>
       </c>
@@ -9719,7 +9720,7 @@
       <c r="AI95" s="2"/>
       <c r="AJ95" s="2"/>
     </row>
-    <row r="96" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>154</v>
       </c>
@@ -9793,7 +9794,7 @@
       <c r="AI96" s="2"/>
       <c r="AJ96" s="2"/>
     </row>
-    <row r="97" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>136</v>
       </c>
@@ -9867,7 +9868,7 @@
       <c r="AI97" s="2"/>
       <c r="AJ97" s="2"/>
     </row>
-    <row r="98" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>124</v>
       </c>
@@ -9945,7 +9946,7 @@
       <c r="AI98" s="2"/>
       <c r="AJ98" s="2"/>
     </row>
-    <row r="99" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>197</v>
       </c>
@@ -10021,7 +10022,7 @@
       <c r="AI99" s="2"/>
       <c r="AJ99" s="2"/>
     </row>
-    <row r="100" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>182</v>
       </c>
@@ -10111,7 +10112,7 @@
         <v>661.98</v>
       </c>
     </row>
-    <row r="101" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>149</v>
       </c>
@@ -10185,7 +10186,7 @@
       <c r="AI101" s="2"/>
       <c r="AJ101" s="2"/>
     </row>
-    <row r="102" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>116</v>
       </c>
@@ -10279,7 +10280,7 @@
         <v>607.51</v>
       </c>
     </row>
-    <row r="103" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>166</v>
       </c>
@@ -10357,7 +10358,7 @@
       <c r="AI103" s="2"/>
       <c r="AJ103" s="2"/>
     </row>
-    <row r="104" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>160</v>
       </c>
@@ -10433,7 +10434,7 @@
       <c r="AI104" s="2"/>
       <c r="AJ104" s="2"/>
     </row>
-    <row r="105" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>172</v>
       </c>
@@ -10513,7 +10514,7 @@
       <c r="AI105" s="2"/>
       <c r="AJ105" s="2"/>
     </row>
-    <row r="106" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>173</v>
       </c>
@@ -10607,7 +10608,7 @@
       <c r="AI106" s="2"/>
       <c r="AJ106" s="2"/>
     </row>
-    <row r="107" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>153</v>
       </c>
@@ -10681,7 +10682,7 @@
       <c r="AI107" s="2"/>
       <c r="AJ107" s="2"/>
     </row>
-    <row r="108" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>156</v>
       </c>
@@ -10771,7 +10772,7 @@
         <v>770.89</v>
       </c>
     </row>
-    <row r="109" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>201</v>
       </c>
@@ -10861,7 +10862,7 @@
       <c r="AI109" s="2"/>
       <c r="AJ109" s="2"/>
     </row>
-    <row r="110" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>325</v>
       </c>
@@ -10949,7 +10950,7 @@
         <v>874.54</v>
       </c>
     </row>
-    <row r="111" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>167</v>
       </c>
@@ -11041,7 +11042,7 @@
       <c r="AI111" s="2"/>
       <c r="AJ111" s="2"/>
     </row>
-    <row r="112" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>168</v>
       </c>
@@ -11127,7 +11128,7 @@
         <v>553.38</v>
       </c>
     </row>
-    <row r="113" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>165</v>
       </c>
@@ -11201,7 +11202,7 @@
       <c r="AI113" s="2"/>
       <c r="AJ113" s="2"/>
     </row>
-    <row r="114" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>155</v>
       </c>
@@ -11287,7 +11288,7 @@
       <c r="AI114" s="2"/>
       <c r="AJ114" s="2"/>
     </row>
-    <row r="115" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>204</v>
       </c>
@@ -11365,7 +11366,7 @@
       <c r="AI115" s="2"/>
       <c r="AJ115" s="2"/>
     </row>
-    <row r="116" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>252</v>
       </c>
@@ -11445,7 +11446,7 @@
       <c r="AI116" s="2"/>
       <c r="AJ116" s="2"/>
     </row>
-    <row r="117" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>139</v>
       </c>
@@ -11527,7 +11528,7 @@
       <c r="AI117" s="2"/>
       <c r="AJ117" s="2"/>
     </row>
-    <row r="118" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>169</v>
       </c>
@@ -11601,7 +11602,7 @@
       <c r="AI118" s="2"/>
       <c r="AJ118" s="2"/>
     </row>
-    <row r="119" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>177</v>
       </c>
@@ -11681,7 +11682,7 @@
       <c r="AI119" s="2"/>
       <c r="AJ119" s="2"/>
     </row>
-    <row r="120" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>74</v>
       </c>
@@ -11755,7 +11756,7 @@
       <c r="AI120" s="2"/>
       <c r="AJ120" s="2"/>
     </row>
-    <row r="121" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>224</v>
       </c>
@@ -11831,7 +11832,7 @@
       <c r="AI121" s="2"/>
       <c r="AJ121" s="2"/>
     </row>
-    <row r="122" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>174</v>
       </c>
@@ -11925,7 +11926,7 @@
         <v>417.13</v>
       </c>
     </row>
-    <row r="123" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>184</v>
       </c>
@@ -12013,7 +12014,7 @@
       <c r="AI123" s="2"/>
       <c r="AJ123" s="2"/>
     </row>
-    <row r="124" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>241</v>
       </c>
@@ -12089,7 +12090,7 @@
       <c r="AI124" s="2"/>
       <c r="AJ124" s="2"/>
     </row>
-    <row r="125" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>216</v>
       </c>
@@ -12165,7 +12166,7 @@
       <c r="AI125" s="2"/>
       <c r="AJ125" s="2"/>
     </row>
-    <row r="126" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>171</v>
       </c>
@@ -12257,7 +12258,7 @@
         <v>795.56</v>
       </c>
     </row>
-    <row r="127" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>228</v>
       </c>
@@ -12335,7 +12336,7 @@
       <c r="AI127" s="2"/>
       <c r="AJ127" s="2"/>
     </row>
-    <row r="128" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>159</v>
       </c>
@@ -12409,7 +12410,7 @@
       <c r="AI128" s="2"/>
       <c r="AJ128" s="2"/>
     </row>
-    <row r="129" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>292</v>
       </c>
@@ -12497,7 +12498,7 @@
       <c r="AI129" s="2"/>
       <c r="AJ129" s="2"/>
     </row>
-    <row r="130" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>207</v>
       </c>
@@ -12591,7 +12592,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="131" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>270</v>
       </c>
@@ -12681,7 +12682,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="132" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>128</v>
       </c>
@@ -12789,7 +12790,7 @@
       </c>
       <c r="AJ132" s="2"/>
     </row>
-    <row r="133" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>147</v>
       </c>
@@ -12877,7 +12878,7 @@
       <c r="AI133" s="2"/>
       <c r="AJ133" s="2"/>
     </row>
-    <row r="134" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>183</v>
       </c>
@@ -12965,7 +12966,7 @@
       </c>
       <c r="AJ134" s="2"/>
     </row>
-    <row r="135" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>144</v>
       </c>
@@ -13039,7 +13040,7 @@
       <c r="AI135" s="2"/>
       <c r="AJ135" s="2"/>
     </row>
-    <row r="136" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>164</v>
       </c>
@@ -13115,7 +13116,7 @@
       <c r="AI136" s="2"/>
       <c r="AJ136" s="2"/>
     </row>
-    <row r="137" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>170</v>
       </c>
@@ -13207,7 +13208,7 @@
         <v>599.79999999999995</v>
       </c>
     </row>
-    <row r="138" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>248</v>
       </c>
@@ -13285,7 +13286,7 @@
       <c r="AI138" s="2"/>
       <c r="AJ138" s="2"/>
     </row>
-    <row r="139" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>142</v>
       </c>
@@ -13375,7 +13376,7 @@
         <v>441.13</v>
       </c>
     </row>
-    <row r="140" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>188</v>
       </c>
@@ -13467,7 +13468,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="141" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>285</v>
       </c>
@@ -13551,7 +13552,7 @@
       <c r="AI141" s="2"/>
       <c r="AJ141" s="2"/>
     </row>
-    <row r="142" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>211</v>
       </c>
@@ -13625,7 +13626,7 @@
       <c r="AI142" s="2"/>
       <c r="AJ142" s="2"/>
     </row>
-    <row r="143" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>261</v>
       </c>
@@ -13717,7 +13718,7 @@
         <v>670.61</v>
       </c>
     </row>
-    <row r="144" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>251</v>
       </c>
@@ -13801,7 +13802,7 @@
       <c r="AI144" s="2"/>
       <c r="AJ144" s="2"/>
     </row>
-    <row r="145" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>220</v>
       </c>
@@ -13893,7 +13894,7 @@
         <v>483.3</v>
       </c>
     </row>
-    <row r="146" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>413</v>
       </c>
@@ -13985,7 +13986,7 @@
         <v>350.14</v>
       </c>
     </row>
-    <row r="147" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>221</v>
       </c>
@@ -14073,7 +14074,7 @@
       <c r="AI147" s="2"/>
       <c r="AJ147" s="2"/>
     </row>
-    <row r="148" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>388</v>
       </c>
@@ -14147,7 +14148,7 @@
       <c r="AI148" s="2"/>
       <c r="AJ148" s="2"/>
     </row>
-    <row r="149" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>214</v>
       </c>
@@ -14237,7 +14238,7 @@
       <c r="AI149" s="2"/>
       <c r="AJ149" s="2"/>
     </row>
-    <row r="150" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>264</v>
       </c>
@@ -14313,7 +14314,7 @@
       <c r="AI150" s="2"/>
       <c r="AJ150" s="2"/>
     </row>
-    <row r="151" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>191</v>
       </c>
@@ -14389,7 +14390,7 @@
       <c r="AI151" s="2"/>
       <c r="AJ151" s="2"/>
     </row>
-    <row r="152" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>200</v>
       </c>
@@ -14479,7 +14480,7 @@
         <v>416.26</v>
       </c>
     </row>
-    <row r="153" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>250</v>
       </c>
@@ -14571,7 +14572,7 @@
         <v>528.27</v>
       </c>
     </row>
-    <row r="154" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>180</v>
       </c>
@@ -14645,7 +14646,7 @@
       <c r="AI154" s="2"/>
       <c r="AJ154" s="2"/>
     </row>
-    <row r="155" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>236</v>
       </c>
@@ -14733,7 +14734,7 @@
       <c r="AI155" s="2"/>
       <c r="AJ155" s="2"/>
     </row>
-    <row r="156" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>232</v>
       </c>
@@ -14821,7 +14822,7 @@
       <c r="AI156" s="2"/>
       <c r="AJ156" s="2"/>
     </row>
-    <row r="157" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>198</v>
       </c>
@@ -14907,7 +14908,7 @@
         <v>451.16</v>
       </c>
     </row>
-    <row r="158" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>175</v>
       </c>
@@ -14983,7 +14984,7 @@
       <c r="AI158" s="2"/>
       <c r="AJ158" s="2"/>
     </row>
-    <row r="159" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>205</v>
       </c>
@@ -15059,7 +15060,7 @@
       <c r="AI159" s="2"/>
       <c r="AJ159" s="2"/>
     </row>
-    <row r="160" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>243</v>
       </c>
@@ -15143,7 +15144,7 @@
       <c r="AI160" s="2"/>
       <c r="AJ160" s="2"/>
     </row>
-    <row r="161" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>238</v>
       </c>
@@ -15231,7 +15232,7 @@
         <v>444.1</v>
       </c>
     </row>
-    <row r="162" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>212</v>
       </c>
@@ -15323,7 +15324,7 @@
         <v>506.91</v>
       </c>
     </row>
-    <row r="163" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>222</v>
       </c>
@@ -15405,7 +15406,7 @@
       <c r="AI163" s="2"/>
       <c r="AJ163" s="2"/>
     </row>
-    <row r="164" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>209</v>
       </c>
@@ -15481,7 +15482,7 @@
       <c r="AI164" s="2"/>
       <c r="AJ164" s="2"/>
     </row>
-    <row r="165" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>274</v>
       </c>
@@ -15557,7 +15558,7 @@
       <c r="AI165" s="2"/>
       <c r="AJ165" s="2"/>
     </row>
-    <row r="166" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>257</v>
       </c>
@@ -15643,7 +15644,7 @@
       <c r="AI166" s="2"/>
       <c r="AJ166" s="2"/>
     </row>
-    <row r="167" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>272</v>
       </c>
@@ -15733,7 +15734,7 @@
       <c r="AI167" s="2"/>
       <c r="AJ167" s="2"/>
     </row>
-    <row r="168" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>98</v>
       </c>
@@ -15807,7 +15808,7 @@
       <c r="AI168" s="2"/>
       <c r="AJ168" s="2"/>
     </row>
-    <row r="169" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>152</v>
       </c>
@@ -15897,7 +15898,7 @@
         <v>462.03</v>
       </c>
     </row>
-    <row r="170" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>227</v>
       </c>
@@ -15993,7 +15994,7 @@
         <v>376.31</v>
       </c>
     </row>
-    <row r="171" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>259</v>
       </c>
@@ -16083,7 +16084,7 @@
       <c r="AI171" s="2"/>
       <c r="AJ171" s="2"/>
     </row>
-    <row r="172" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>263</v>
       </c>
@@ -16167,7 +16168,7 @@
       <c r="AI172" s="2"/>
       <c r="AJ172" s="2"/>
     </row>
-    <row r="173" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>233</v>
       </c>
@@ -16255,7 +16256,7 @@
       <c r="AI173" s="2"/>
       <c r="AJ173" s="2"/>
     </row>
-    <row r="174" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>187</v>
       </c>
@@ -16349,7 +16350,7 @@
       <c r="AI174" s="2"/>
       <c r="AJ174" s="2"/>
     </row>
-    <row r="175" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>378</v>
       </c>
@@ -16437,7 +16438,7 @@
       <c r="AI175" s="2"/>
       <c r="AJ175" s="2"/>
     </row>
-    <row r="176" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>415</v>
       </c>
@@ -16529,7 +16530,7 @@
         <v>431.44</v>
       </c>
     </row>
-    <row r="177" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>225</v>
       </c>
@@ -16617,7 +16618,7 @@
       <c r="AI177" s="2"/>
       <c r="AJ177" s="2"/>
     </row>
-    <row r="178" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>231</v>
       </c>
@@ -16693,7 +16694,7 @@
       <c r="AI178" s="2"/>
       <c r="AJ178" s="2"/>
     </row>
-    <row r="179" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>192</v>
       </c>
@@ -16779,7 +16780,7 @@
         <v>396.92</v>
       </c>
     </row>
-    <row r="180" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>277</v>
       </c>
@@ -16855,7 +16856,7 @@
       <c r="AI180" s="2"/>
       <c r="AJ180" s="2"/>
     </row>
-    <row r="181" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>176</v>
       </c>
@@ -16947,7 +16948,7 @@
         <v>498.2</v>
       </c>
     </row>
-    <row r="182" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>390</v>
       </c>
@@ -17039,7 +17040,7 @@
         <v>280.45</v>
       </c>
     </row>
-    <row r="183" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>262</v>
       </c>
@@ -17119,7 +17120,7 @@
       <c r="AI183" s="2"/>
       <c r="AJ183" s="2"/>
     </row>
-    <row r="184" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>249</v>
       </c>
@@ -17193,7 +17194,7 @@
       <c r="AI184" s="2"/>
       <c r="AJ184" s="2"/>
     </row>
-    <row r="185" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>295</v>
       </c>
@@ -17279,7 +17280,7 @@
       <c r="AI185" s="2"/>
       <c r="AJ185" s="2"/>
     </row>
-    <row r="186" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>288</v>
       </c>
@@ -17357,7 +17358,7 @@
       <c r="AI186" s="2"/>
       <c r="AJ186" s="2"/>
     </row>
-    <row r="187" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>230</v>
       </c>
@@ -17431,7 +17432,7 @@
       <c r="AI187" s="2"/>
       <c r="AJ187" s="2"/>
     </row>
-    <row r="188" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>283</v>
       </c>
@@ -17505,7 +17506,7 @@
       <c r="AI188" s="2"/>
       <c r="AJ188" s="2"/>
     </row>
-    <row r="189" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>246</v>
       </c>
@@ -17595,7 +17596,7 @@
         <v>445.91</v>
       </c>
     </row>
-    <row r="190" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
         <v>265</v>
       </c>
@@ -17671,7 +17672,7 @@
       <c r="AI190" s="2"/>
       <c r="AJ190" s="2"/>
     </row>
-    <row r="191" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>260</v>
       </c>
@@ -17753,7 +17754,7 @@
       <c r="AI191" s="2"/>
       <c r="AJ191" s="2"/>
     </row>
-    <row r="192" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
         <v>280</v>
       </c>
@@ -17841,7 +17842,7 @@
       <c r="AI192" s="2"/>
       <c r="AJ192" s="2"/>
     </row>
-    <row r="193" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
         <v>346</v>
       </c>
@@ -17919,7 +17920,7 @@
       <c r="AI193" s="2"/>
       <c r="AJ193" s="2"/>
     </row>
-    <row r="194" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
         <v>206</v>
       </c>
@@ -18011,7 +18012,7 @@
         <v>430.42</v>
       </c>
     </row>
-    <row r="195" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
         <v>226</v>
       </c>
@@ -18085,7 +18086,7 @@
       <c r="AI195" s="2"/>
       <c r="AJ195" s="2"/>
     </row>
-    <row r="196" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
         <v>245</v>
       </c>
@@ -18171,7 +18172,7 @@
       <c r="AI196" s="2"/>
       <c r="AJ196" s="2"/>
     </row>
-    <row r="197" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
         <v>271</v>
       </c>
@@ -18259,7 +18260,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="198" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
         <v>414</v>
       </c>
@@ -18333,7 +18334,7 @@
       <c r="AI198" s="2"/>
       <c r="AJ198" s="2"/>
     </row>
-    <row r="199" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
         <v>239</v>
       </c>
@@ -18411,7 +18412,7 @@
       <c r="AI199" s="2"/>
       <c r="AJ199" s="2"/>
     </row>
-    <row r="200" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>123</v>
       </c>
@@ -18487,7 +18488,7 @@
       <c r="AI200" s="2"/>
       <c r="AJ200" s="2"/>
     </row>
-    <row r="201" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>235</v>
       </c>
@@ -18575,7 +18576,7 @@
         <v>284.17</v>
       </c>
     </row>
-    <row r="202" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>275</v>
       </c>
@@ -18665,7 +18666,7 @@
         <v>334.73</v>
       </c>
     </row>
-    <row r="203" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>307</v>
       </c>
@@ -18741,7 +18742,7 @@
       <c r="AI203" s="2"/>
       <c r="AJ203" s="2"/>
     </row>
-    <row r="204" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>329</v>
       </c>
@@ -18819,7 +18820,7 @@
       <c r="AI204" s="2"/>
       <c r="AJ204" s="2"/>
     </row>
-    <row r="205" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>304</v>
       </c>
@@ -18903,7 +18904,7 @@
       <c r="AI205" s="2"/>
       <c r="AJ205" s="2"/>
     </row>
-    <row r="206" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>389</v>
       </c>
@@ -18977,7 +18978,7 @@
       <c r="AI206" s="2"/>
       <c r="AJ206" s="2"/>
     </row>
-    <row r="207" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>269</v>
       </c>
@@ -19073,7 +19074,7 @@
         <v>376.48</v>
       </c>
     </row>
-    <row r="208" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>416</v>
       </c>
@@ -19163,7 +19164,7 @@
         <v>497.71</v>
       </c>
     </row>
-    <row r="209" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>267</v>
       </c>
@@ -19249,7 +19250,7 @@
         <v>286.95</v>
       </c>
     </row>
-    <row r="210" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>279</v>
       </c>
@@ -19341,7 +19342,7 @@
       <c r="AI210" s="2"/>
       <c r="AJ210" s="2"/>
     </row>
-    <row r="211" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>223</v>
       </c>
@@ -19415,7 +19416,7 @@
       <c r="AI211" s="2"/>
       <c r="AJ211" s="2"/>
     </row>
-    <row r="212" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>391</v>
       </c>
@@ -19495,7 +19496,7 @@
       <c r="AI212" s="2"/>
       <c r="AJ212" s="2"/>
     </row>
-    <row r="213" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
         <v>305</v>
       </c>
@@ -19583,7 +19584,7 @@
       <c r="AI213" s="2"/>
       <c r="AJ213" s="2"/>
     </row>
-    <row r="214" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
         <v>266</v>
       </c>
@@ -19669,7 +19670,7 @@
       <c r="AI214" s="2"/>
       <c r="AJ214" s="2"/>
     </row>
-    <row r="215" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
         <v>210</v>
       </c>
@@ -19757,7 +19758,7 @@
       <c r="AI215" s="2"/>
       <c r="AJ215" s="2"/>
     </row>
-    <row r="216" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>145</v>
       </c>
@@ -19831,7 +19832,7 @@
       <c r="AI216" s="2"/>
       <c r="AJ216" s="2"/>
     </row>
-    <row r="217" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>290</v>
       </c>
@@ -19905,7 +19906,7 @@
       <c r="AI217" s="2"/>
       <c r="AJ217" s="2"/>
     </row>
-    <row r="218" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>215</v>
       </c>
@@ -19993,7 +19994,7 @@
       <c r="AI218" s="2"/>
       <c r="AJ218" s="2"/>
     </row>
-    <row r="219" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>297</v>
       </c>
@@ -20081,7 +20082,7 @@
       <c r="AI219" s="2"/>
       <c r="AJ219" s="2"/>
     </row>
-    <row r="220" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
         <v>276</v>
       </c>
@@ -20173,7 +20174,7 @@
         <v>238.52</v>
       </c>
     </row>
-    <row r="221" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>312</v>
       </c>
@@ -20265,7 +20266,7 @@
         <v>434.27</v>
       </c>
     </row>
-    <row r="222" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
         <v>161</v>
       </c>
@@ -20355,7 +20356,7 @@
       <c r="AI222" s="2"/>
       <c r="AJ222" s="2"/>
     </row>
-    <row r="223" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
         <v>282</v>
       </c>
@@ -20447,7 +20448,7 @@
         <v>229.35</v>
       </c>
     </row>
-    <row r="224" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
         <v>337</v>
       </c>
@@ -20607,7 +20608,7 @@
       <c r="AI225" s="2"/>
       <c r="AJ225" s="2"/>
     </row>
-    <row r="226" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>323</v>
       </c>
@@ -20697,7 +20698,7 @@
         <v>299.83</v>
       </c>
     </row>
-    <row r="227" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
         <v>256</v>
       </c>
@@ -20783,7 +20784,7 @@
         <v>125.4</v>
       </c>
     </row>
-    <row r="228" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
         <v>317</v>
       </c>
@@ -20863,7 +20864,7 @@
       <c r="AI228" s="2"/>
       <c r="AJ228" s="2"/>
     </row>
-    <row r="229" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
         <v>202</v>
       </c>
@@ -20941,7 +20942,7 @@
       <c r="AI229" s="2"/>
       <c r="AJ229" s="2"/>
     </row>
-    <row r="230" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>141</v>
       </c>
@@ -21031,7 +21032,7 @@
       <c r="AI230" s="2"/>
       <c r="AJ230" s="2"/>
     </row>
-    <row r="231" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
         <v>315</v>
       </c>
@@ -21119,7 +21120,7 @@
       <c r="AI231" s="2"/>
       <c r="AJ231" s="2"/>
     </row>
-    <row r="232" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
         <v>258</v>
       </c>
@@ -21205,7 +21206,7 @@
         <v>256.38</v>
       </c>
     </row>
-    <row r="233" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
         <v>293</v>
       </c>
@@ -21291,7 +21292,7 @@
       <c r="AI233" s="2"/>
       <c r="AJ233" s="2"/>
     </row>
-    <row r="234" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
         <v>318</v>
       </c>
@@ -21383,7 +21384,7 @@
         <v>180.7</v>
       </c>
     </row>
-    <row r="235" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
         <v>298</v>
       </c>
@@ -21475,7 +21476,7 @@
         <v>294.72000000000003</v>
       </c>
     </row>
-    <row r="236" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
         <v>255</v>
       </c>
@@ -21565,7 +21566,7 @@
         <v>294.62</v>
       </c>
     </row>
-    <row r="237" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
         <v>284</v>
       </c>
@@ -21655,7 +21656,7 @@
         <v>193.5</v>
       </c>
     </row>
-    <row r="238" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
         <v>289</v>
       </c>
@@ -21743,7 +21744,7 @@
       <c r="AI238" s="2"/>
       <c r="AJ238" s="2"/>
     </row>
-    <row r="239" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
         <v>376</v>
       </c>
@@ -21833,7 +21834,7 @@
         <v>216.51</v>
       </c>
     </row>
-    <row r="240" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
         <v>332</v>
       </c>
@@ -21921,7 +21922,7 @@
         <v>213.8</v>
       </c>
     </row>
-    <row r="241" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>330</v>
       </c>
@@ -22013,7 +22014,7 @@
         <v>185.65</v>
       </c>
     </row>
-    <row r="242" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
         <v>331</v>
       </c>
@@ -22087,7 +22088,7 @@
       <c r="AI242" s="2"/>
       <c r="AJ242" s="2"/>
     </row>
-    <row r="243" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>340</v>
       </c>
@@ -22169,7 +22170,7 @@
       <c r="AI243" s="2"/>
       <c r="AJ243" s="2"/>
     </row>
-    <row r="244" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>287</v>
       </c>
@@ -22261,7 +22262,7 @@
         <v>220.19</v>
       </c>
     </row>
-    <row r="245" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>339</v>
       </c>
@@ -22341,7 +22342,7 @@
       <c r="AI245" s="2"/>
       <c r="AJ245" s="2"/>
     </row>
-    <row r="246" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
         <v>308</v>
       </c>
@@ -22431,7 +22432,7 @@
       <c r="AI246" s="2"/>
       <c r="AJ246" s="2"/>
     </row>
-    <row r="247" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
         <v>306</v>
       </c>
@@ -22507,7 +22508,7 @@
       <c r="AI247" s="2"/>
       <c r="AJ247" s="2"/>
     </row>
-    <row r="248" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>336</v>
       </c>
@@ -22583,7 +22584,7 @@
       <c r="AI248" s="2"/>
       <c r="AJ248" s="2"/>
     </row>
-    <row r="249" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>300</v>
       </c>
@@ -22673,7 +22674,7 @@
       <c r="AI249" s="2"/>
       <c r="AJ249" s="2"/>
     </row>
-    <row r="250" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>253</v>
       </c>
@@ -22751,7 +22752,7 @@
       <c r="AI250" s="2"/>
       <c r="AJ250" s="2"/>
     </row>
-    <row r="251" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>383</v>
       </c>
@@ -22823,7 +22824,7 @@
       <c r="AI251" s="2"/>
       <c r="AJ251" s="2"/>
     </row>
-    <row r="252" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>314</v>
       </c>
@@ -22901,7 +22902,7 @@
       <c r="AI252" s="2"/>
       <c r="AJ252" s="2"/>
     </row>
-    <row r="253" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>334</v>
       </c>
@@ -22991,7 +22992,7 @@
         <v>99.85</v>
       </c>
     </row>
-    <row r="254" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>294</v>
       </c>
@@ -23081,7 +23082,7 @@
       <c r="AI254" s="2"/>
       <c r="AJ254" s="2"/>
     </row>
-    <row r="255" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>412</v>
       </c>
@@ -23171,7 +23172,7 @@
         <v>120.79</v>
       </c>
     </row>
-    <row r="256" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>291</v>
       </c>
@@ -23263,7 +23264,7 @@
         <v>204.32</v>
       </c>
     </row>
-    <row r="257" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>342</v>
       </c>
@@ -23353,7 +23354,7 @@
         <v>186.94</v>
       </c>
     </row>
-    <row r="258" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>353</v>
       </c>
@@ -23445,7 +23446,7 @@
         <v>212.63</v>
       </c>
     </row>
-    <row r="259" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>237</v>
       </c>
@@ -23519,7 +23520,7 @@
       <c r="AI259" s="2"/>
       <c r="AJ259" s="2"/>
     </row>
-    <row r="260" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
         <v>417</v>
       </c>
@@ -23607,7 +23608,7 @@
         <v>223.53</v>
       </c>
     </row>
-    <row r="261" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>190</v>
       </c>
@@ -23695,7 +23696,7 @@
       <c r="AI261" s="2"/>
       <c r="AJ261" s="2"/>
     </row>
-    <row r="262" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>179</v>
       </c>
@@ -23769,7 +23770,7 @@
       <c r="AI262" s="2"/>
       <c r="AJ262" s="2"/>
     </row>
-    <row r="263" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>218</v>
       </c>
@@ -23847,7 +23848,7 @@
       <c r="AI263" s="2"/>
       <c r="AJ263" s="2"/>
     </row>
-    <row r="264" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>234</v>
       </c>
@@ -23921,7 +23922,7 @@
       <c r="AI264" s="2"/>
       <c r="AJ264" s="2"/>
     </row>
-    <row r="265" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>247</v>
       </c>
@@ -24015,7 +24016,7 @@
       <c r="AI265" s="2"/>
       <c r="AJ265" s="2"/>
     </row>
-    <row r="266" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>377</v>
       </c>
@@ -24109,7 +24110,7 @@
         <v>139.6</v>
       </c>
     </row>
-    <row r="267" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>384</v>
       </c>
@@ -24181,7 +24182,7 @@
       <c r="AI267" s="2"/>
       <c r="AJ267" s="2"/>
     </row>
-    <row r="268" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>296</v>
       </c>
@@ -24273,7 +24274,7 @@
       <c r="AI268" s="2"/>
       <c r="AJ268" s="2"/>
     </row>
-    <row r="269" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>242</v>
       </c>
@@ -24353,7 +24354,7 @@
       <c r="AI269" s="2"/>
       <c r="AJ269" s="2"/>
     </row>
-    <row r="270" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>219</v>
       </c>
@@ -24427,7 +24428,7 @@
       <c r="AI270" s="2"/>
       <c r="AJ270" s="2"/>
     </row>
-    <row r="271" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>380</v>
       </c>
@@ -24517,7 +24518,7 @@
         <v>223.82</v>
       </c>
     </row>
-    <row r="272" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>309</v>
       </c>
@@ -24607,7 +24608,7 @@
         <v>220.8</v>
       </c>
     </row>
-    <row r="273" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>345</v>
       </c>
@@ -24683,7 +24684,7 @@
       <c r="AI273" s="2"/>
       <c r="AJ273" s="2"/>
     </row>
-    <row r="274" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>338</v>
       </c>
@@ -24757,7 +24758,7 @@
       <c r="AI274" s="2"/>
       <c r="AJ274" s="2"/>
     </row>
-    <row r="275" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>321</v>
       </c>
@@ -24865,7 +24866,7 @@
       </c>
       <c r="AJ275" s="2"/>
     </row>
-    <row r="276" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>382</v>
       </c>
@@ -24937,7 +24938,7 @@
       <c r="AI276" s="2"/>
       <c r="AJ276" s="2"/>
     </row>
-    <row r="277" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>303</v>
       </c>
@@ -25033,7 +25034,7 @@
         <v>239.28</v>
       </c>
     </row>
-    <row r="278" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>392</v>
       </c>
@@ -25125,7 +25126,7 @@
         <v>146.82</v>
       </c>
     </row>
-    <row r="279" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>268</v>
       </c>
@@ -25199,7 +25200,7 @@
       <c r="AI279" s="2"/>
       <c r="AJ279" s="2"/>
     </row>
-    <row r="280" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>348</v>
       </c>
@@ -25277,7 +25278,7 @@
       <c r="AI280" s="2"/>
       <c r="AJ280" s="2"/>
     </row>
-    <row r="281" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>385</v>
       </c>
@@ -25349,7 +25350,7 @@
       <c r="AI281" s="2"/>
       <c r="AJ281" s="2"/>
     </row>
-    <row r="282" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
         <v>324</v>
       </c>
@@ -25429,7 +25430,7 @@
       <c r="AI282" s="2"/>
       <c r="AJ282" s="2"/>
     </row>
-    <row r="283" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>327</v>
       </c>
@@ -25521,7 +25522,7 @@
         <v>136.74</v>
       </c>
     </row>
-    <row r="284" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>341</v>
       </c>
@@ -25609,7 +25610,7 @@
       <c r="AI284" s="2"/>
       <c r="AJ284" s="2"/>
     </row>
-    <row r="285" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>310</v>
       </c>
@@ -25701,7 +25702,7 @@
         <v>128.94</v>
       </c>
     </row>
-    <row r="286" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>352</v>
       </c>
@@ -25789,7 +25790,7 @@
       <c r="AI286" s="2"/>
       <c r="AJ286" s="2"/>
     </row>
-    <row r="287" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>379</v>
       </c>
@@ -25881,7 +25882,7 @@
         <v>179.95</v>
       </c>
     </row>
-    <row r="288" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>311</v>
       </c>
@@ -25955,7 +25956,7 @@
       <c r="AI288" s="2"/>
       <c r="AJ288" s="2"/>
     </row>
-    <row r="289" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>273</v>
       </c>
@@ -26045,7 +26046,7 @@
       <c r="AI289" s="2"/>
       <c r="AJ289" s="2"/>
     </row>
-    <row r="290" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>254</v>
       </c>
@@ -26139,7 +26140,7 @@
       <c r="AI290" s="2"/>
       <c r="AJ290" s="2"/>
     </row>
-    <row r="291" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>328</v>
       </c>
@@ -26219,7 +26220,7 @@
       <c r="AI291" s="2"/>
       <c r="AJ291" s="2"/>
     </row>
-    <row r="292" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
         <v>355</v>
       </c>
@@ -26311,7 +26312,7 @@
         <v>134.49</v>
       </c>
     </row>
-    <row r="293" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>347</v>
       </c>
@@ -26389,7 +26390,7 @@
       <c r="AI293" s="2"/>
       <c r="AJ293" s="2"/>
     </row>
-    <row r="294" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>322</v>
       </c>
@@ -26463,7 +26464,7 @@
       <c r="AI294" s="2"/>
       <c r="AJ294" s="2"/>
     </row>
-    <row r="295" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
         <v>343</v>
       </c>
@@ -26555,7 +26556,7 @@
         <v>203.58</v>
       </c>
     </row>
-    <row r="296" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>393</v>
       </c>
@@ -26633,7 +26634,7 @@
       <c r="AI296" s="2"/>
       <c r="AJ296" s="2"/>
     </row>
-    <row r="297" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>316</v>
       </c>
@@ -26707,7 +26708,7 @@
       <c r="AI297" s="2"/>
       <c r="AJ297" s="2"/>
     </row>
-    <row r="298" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>410</v>
       </c>
@@ -26799,7 +26800,7 @@
         <v>126.28</v>
       </c>
     </row>
-    <row r="299" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>240</v>
       </c>
@@ -26891,7 +26892,7 @@
       <c r="AI299" s="2"/>
       <c r="AJ299" s="2"/>
     </row>
-    <row r="300" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
         <v>411</v>
       </c>
@@ -26981,7 +26982,7 @@
         <v>98.38</v>
       </c>
     </row>
-    <row r="301" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
         <v>404</v>
       </c>
@@ -27065,7 +27066,7 @@
       <c r="AI301" s="2"/>
       <c r="AJ301" s="2"/>
     </row>
-    <row r="302" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
         <v>349</v>
       </c>
@@ -27155,7 +27156,7 @@
       <c r="AI302" s="2"/>
       <c r="AJ302" s="2"/>
     </row>
-    <row r="303" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
         <v>301</v>
       </c>
@@ -27233,7 +27234,7 @@
       <c r="AI303" s="2"/>
       <c r="AJ303" s="2"/>
     </row>
-    <row r="304" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
         <v>302</v>
       </c>
@@ -27295,7 +27296,7 @@
       <c r="AI304" s="2"/>
       <c r="AJ304" s="2"/>
     </row>
-    <row r="305" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
         <v>360</v>
       </c>
@@ -27385,7 +27386,7 @@
         <v>251.78</v>
       </c>
     </row>
-    <row r="306" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
         <v>320</v>
       </c>
@@ -27477,7 +27478,7 @@
         <v>178.26</v>
       </c>
     </row>
-    <row r="307" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
         <v>356</v>
       </c>
@@ -27557,7 +27558,7 @@
       <c r="AI307" s="2"/>
       <c r="AJ307" s="2"/>
     </row>
-    <row r="308" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
         <v>359</v>
       </c>
@@ -27645,7 +27646,7 @@
         <v>105.03</v>
       </c>
     </row>
-    <row r="309" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
         <v>350</v>
       </c>
@@ -27721,7 +27722,7 @@
       <c r="AI309" s="2"/>
       <c r="AJ309" s="2"/>
     </row>
-    <row r="310" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
         <v>387</v>
       </c>
@@ -27811,7 +27812,7 @@
         <v>179.95</v>
       </c>
     </row>
-    <row r="311" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
         <v>358</v>
       </c>
@@ -27883,7 +27884,7 @@
       <c r="AI311" s="2"/>
       <c r="AJ311" s="2"/>
     </row>
-    <row r="312" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A312" s="2" t="s">
         <v>402</v>
       </c>
@@ -27975,7 +27976,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="313" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
         <v>357</v>
       </c>
@@ -28065,7 +28066,7 @@
       <c r="AI313" s="2"/>
       <c r="AJ313" s="2"/>
     </row>
-    <row r="314" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
         <v>422</v>
       </c>
@@ -28137,7 +28138,7 @@
       <c r="AI314" s="2"/>
       <c r="AJ314" s="2"/>
     </row>
-    <row r="315" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
         <v>420</v>
       </c>
@@ -28209,7 +28210,7 @@
       <c r="AI315" s="2"/>
       <c r="AJ315" s="2"/>
     </row>
-    <row r="316" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
         <v>418</v>
       </c>
@@ -28293,7 +28294,7 @@
         <v>128.69999999999999</v>
       </c>
     </row>
-    <row r="317" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A317" s="2" t="s">
         <v>396</v>
       </c>
@@ -28367,7 +28368,7 @@
       <c r="AI317" s="2"/>
       <c r="AJ317" s="2"/>
     </row>
-    <row r="318" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
         <v>361</v>
       </c>
@@ -28447,7 +28448,7 @@
       <c r="AI318" s="2"/>
       <c r="AJ318" s="2"/>
     </row>
-    <row r="319" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
         <v>326</v>
       </c>
@@ -28521,7 +28522,7 @@
       <c r="AI319" s="2"/>
       <c r="AJ319" s="2"/>
     </row>
-    <row r="320" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
         <v>364</v>
       </c>
@@ -28611,7 +28612,7 @@
       <c r="AI320" s="2"/>
       <c r="AJ320" s="2"/>
     </row>
-    <row r="321" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
         <v>344</v>
       </c>
@@ -28683,7 +28684,7 @@
       <c r="AI321" s="2"/>
       <c r="AJ321" s="2"/>
     </row>
-    <row r="322" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A322" s="2" t="s">
         <v>351</v>
       </c>
@@ -28755,7 +28756,7 @@
       <c r="AI322" s="2"/>
       <c r="AJ322" s="2"/>
     </row>
-    <row r="323" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A323" s="2" t="s">
         <v>319</v>
       </c>
@@ -28829,7 +28830,7 @@
       <c r="AI323" s="2"/>
       <c r="AJ323" s="2"/>
     </row>
-    <row r="324" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A324" s="2" t="s">
         <v>397</v>
       </c>
@@ -28905,7 +28906,7 @@
       <c r="AI324" s="2"/>
       <c r="AJ324" s="2"/>
     </row>
-    <row r="325" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
         <v>354</v>
       </c>
@@ -28977,7 +28978,7 @@
       <c r="AI325" s="2"/>
       <c r="AJ325" s="2"/>
     </row>
-    <row r="326" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
         <v>395</v>
       </c>
@@ -29053,7 +29054,7 @@
       <c r="AI326" s="2"/>
       <c r="AJ326" s="2"/>
     </row>
-    <row r="327" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
         <v>399</v>
       </c>
@@ -29145,7 +29146,7 @@
       <c r="AI327" s="2"/>
       <c r="AJ327" s="2"/>
     </row>
-    <row r="328" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
         <v>333</v>
       </c>
@@ -29219,7 +29220,7 @@
       <c r="AI328" s="2"/>
       <c r="AJ328" s="2"/>
     </row>
-    <row r="329" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
         <v>394</v>
       </c>
@@ -29293,7 +29294,7 @@
       <c r="AI329" s="2"/>
       <c r="AJ329" s="2"/>
     </row>
-    <row r="330" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
         <v>403</v>
       </c>
@@ -29385,7 +29386,7 @@
         <v>111.32</v>
       </c>
     </row>
-    <row r="331" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
         <v>367</v>
       </c>
@@ -29457,7 +29458,7 @@
       <c r="AI331" s="2"/>
       <c r="AJ331" s="2"/>
     </row>
-    <row r="332" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A332" s="2" t="s">
         <v>365</v>
       </c>
@@ -29529,7 +29530,7 @@
       <c r="AI332" s="2"/>
       <c r="AJ332" s="2"/>
     </row>
-    <row r="333" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
         <v>362</v>
       </c>
@@ -29601,7 +29602,7 @@
       <c r="AI333" s="2"/>
       <c r="AJ333" s="2"/>
     </row>
-    <row r="334" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A334" s="2" t="s">
         <v>398</v>
       </c>
@@ -29675,7 +29676,7 @@
       <c r="AI334" s="2"/>
       <c r="AJ334" s="2"/>
     </row>
-    <row r="335" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A335" s="2" t="s">
         <v>371</v>
       </c>
@@ -29765,7 +29766,7 @@
         <v>100.29</v>
       </c>
     </row>
-    <row r="336" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A336" s="2" t="s">
         <v>363</v>
       </c>
@@ -29837,7 +29838,7 @@
       <c r="AI336" s="2"/>
       <c r="AJ336" s="2"/>
     </row>
-    <row r="337" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A337" s="2" t="s">
         <v>407</v>
       </c>
@@ -29917,7 +29918,7 @@
       <c r="AI337" s="2"/>
       <c r="AJ337" s="2"/>
     </row>
-    <row r="338" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
         <v>400</v>
       </c>
@@ -29979,7 +29980,7 @@
       <c r="AI338" s="2"/>
       <c r="AJ338" s="2"/>
     </row>
-    <row r="339" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
         <v>429</v>
       </c>
@@ -30051,7 +30052,7 @@
       <c r="AI339" s="2"/>
       <c r="AJ339" s="2"/>
     </row>
-    <row r="340" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
         <v>366</v>
       </c>
@@ -30123,7 +30124,7 @@
       <c r="AI340" s="2"/>
       <c r="AJ340" s="2"/>
     </row>
-    <row r="341" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
         <v>381</v>
       </c>
@@ -30197,7 +30198,7 @@
       <c r="AI341" s="2"/>
       <c r="AJ341" s="2"/>
     </row>
-    <row r="342" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
         <v>369</v>
       </c>
@@ -30269,7 +30270,7 @@
       <c r="AI342" s="2"/>
       <c r="AJ342" s="2"/>
     </row>
-    <row r="343" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
         <v>406</v>
       </c>
@@ -30355,7 +30356,7 @@
       <c r="AI343" s="2"/>
       <c r="AJ343" s="2"/>
     </row>
-    <row r="344" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
         <v>368</v>
       </c>
@@ -30427,7 +30428,7 @@
       <c r="AI344" s="2"/>
       <c r="AJ344" s="2"/>
     </row>
-    <row r="345" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
         <v>405</v>
       </c>
@@ -30509,7 +30510,7 @@
       <c r="AI345" s="2"/>
       <c r="AJ345" s="2"/>
     </row>
-    <row r="346" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
         <v>425</v>
       </c>
@@ -30581,7 +30582,7 @@
       <c r="AI346" s="2"/>
       <c r="AJ346" s="2"/>
     </row>
-    <row r="347" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
         <v>423</v>
       </c>
@@ -30653,7 +30654,7 @@
       <c r="AI347" s="2"/>
       <c r="AJ347" s="2"/>
     </row>
-    <row r="348" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A348" s="2" t="s">
         <v>409</v>
       </c>
@@ -30745,7 +30746,7 @@
       <c r="AI348" s="2"/>
       <c r="AJ348" s="2"/>
     </row>
-    <row r="349" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
         <v>374</v>
       </c>
@@ -30817,7 +30818,7 @@
       <c r="AI349" s="2"/>
       <c r="AJ349" s="2"/>
     </row>
-    <row r="350" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
         <v>370</v>
       </c>
@@ -30889,7 +30890,7 @@
       <c r="AI350" s="2"/>
       <c r="AJ350" s="2"/>
     </row>
-    <row r="351" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A351" s="2" t="s">
         <v>372</v>
       </c>
@@ -30961,7 +30962,7 @@
       <c r="AI351" s="2"/>
       <c r="AJ351" s="2"/>
     </row>
-    <row r="352" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
         <v>408</v>
       </c>
@@ -31035,7 +31036,7 @@
       <c r="AI352" s="2"/>
       <c r="AJ352" s="2"/>
     </row>
-    <row r="353" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
         <v>373</v>
       </c>
@@ -31107,7 +31108,7 @@
       <c r="AI353" s="2"/>
       <c r="AJ353" s="2"/>
     </row>
-    <row r="354" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A354" s="2" t="s">
         <v>375</v>
       </c>
@@ -31179,7 +31180,7 @@
       <c r="AI354" s="2"/>
       <c r="AJ354" s="2"/>
     </row>
-    <row r="355" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
         <v>118</v>
       </c>
@@ -31247,7 +31248,7 @@
       <c r="AI355" s="2"/>
       <c r="AJ355" s="2"/>
     </row>
-    <row r="356" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
         <v>431</v>
       </c>
@@ -31315,7 +31316,7 @@
       <c r="AI356" s="2"/>
       <c r="AJ356" s="2"/>
     </row>
-    <row r="357" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
         <v>335</v>
       </c>
@@ -31385,7 +31386,7 @@
       <c r="AI357" s="2"/>
       <c r="AJ357" s="2"/>
     </row>
-    <row r="358" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
         <v>313</v>
       </c>
@@ -31453,7 +31454,7 @@
       <c r="AI358" s="2"/>
       <c r="AJ358" s="2"/>
     </row>
-    <row r="359" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
         <v>186</v>
       </c>
@@ -31515,7 +31516,7 @@
       <c r="AI359" s="2"/>
       <c r="AJ359" s="2"/>
     </row>
-    <row r="360" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
         <v>432</v>
       </c>
@@ -31583,7 +31584,7 @@
       <c r="AI360" s="2"/>
       <c r="AJ360" s="2"/>
     </row>
-    <row r="361" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
         <v>278</v>
       </c>
@@ -31651,7 +31652,7 @@
       <c r="AI361" s="2"/>
       <c r="AJ361" s="2"/>
     </row>
-    <row r="362" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
         <v>419</v>
       </c>
@@ -31711,7 +31712,7 @@
       <c r="AI362" s="2"/>
       <c r="AJ362" s="2"/>
     </row>
-    <row r="363" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
         <v>424</v>
       </c>
@@ -31771,7 +31772,7 @@
       <c r="AI363" s="2"/>
       <c r="AJ363" s="2"/>
     </row>
-    <row r="364" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A364" s="2" t="s">
         <v>386</v>
       </c>
@@ -31821,7 +31822,7 @@
       <c r="AI364" s="2"/>
       <c r="AJ364" s="2"/>
     </row>
-    <row r="365" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
         <v>401</v>
       </c>
@@ -31881,7 +31882,7 @@
       <c r="AI365" s="2"/>
       <c r="AJ365" s="2"/>
     </row>
-    <row r="366" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
         <v>421</v>
       </c>
@@ -31929,7 +31930,7 @@
       <c r="AI366" s="2"/>
       <c r="AJ366" s="2"/>
     </row>
-    <row r="367" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
         <v>426</v>
       </c>
@@ -31987,7 +31988,7 @@
       <c r="AI367" s="2"/>
       <c r="AJ367" s="2"/>
     </row>
-    <row r="368" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
         <v>427</v>
       </c>
@@ -32035,7 +32036,7 @@
       <c r="AI368" s="2"/>
       <c r="AJ368" s="2"/>
     </row>
-    <row r="369" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
         <v>428</v>
       </c>
@@ -32083,7 +32084,7 @@
       <c r="AI369" s="2"/>
       <c r="AJ369" s="2"/>
     </row>
-    <row r="370" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:36" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
         <v>430</v>
       </c>
@@ -32132,7 +32133,13 @@
       <c r="AJ370" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ370" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AJ370" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="鄂州市"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>